<commit_message>
arrays c# c++ done
</commit_message>
<xml_diff>
--- a/Blind75Notes.xlsx
+++ b/Blind75Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keanu\Desktop\Programing\Blind75\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keanu/Desktop/Programming/Blind75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9F3096-21D1-400F-A1D3-DA22DE5032C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6EAA7C-FDF8-D446-A29A-6D5431CFBF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20640" yWindow="0" windowWidth="20640" windowHeight="16680" xr2:uid="{E1B74584-583F-9444-8CED-CEB40E695B1C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{E1B74584-583F-9444-8CED-CEB40E695B1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t>Product of Array Except Self</t>
   </si>
   <si>
-    <t>make two passes, from left then from right, to compute products</t>
-  </si>
-  <si>
     <t xml:space="preserve">Encode and Decode Strings </t>
   </si>
   <si>
@@ -279,13 +276,16 @@
   </si>
   <si>
     <t>Bit Manipulation</t>
+  </si>
+  <si>
+    <t>create empty array to store and update values;make two passes, from left then from right, to compute products</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -387,7 +387,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
@@ -396,7 +396,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -717,23 +716,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5327056-F56C-9646-8CAD-3FA69CA8A264}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="218.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="218.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="22.8">
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" customHeight="1">
+    <row r="2" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -744,7 +743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24" customHeight="1">
+    <row r="3" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -755,7 +754,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -766,7 +765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24" customHeight="1">
+    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -777,7 +776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" customHeight="1">
+    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -788,7 +787,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="24" customHeight="1">
+    <row r="7" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
@@ -799,7 +798,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="24" customHeight="1">
+    <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -807,290 +806,288 @@
         <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="24" customHeight="1">
-      <c r="A9" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="24" customHeight="1">
-      <c r="A10" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="24" customHeight="1">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="3" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="24" customHeight="1">
-      <c r="A12" s="4" t="s">
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="24" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="3" t="s">
+    <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="24" customHeight="1">
-      <c r="A14" s="2" t="s">
+      <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24" customHeight="1">
-      <c r="A15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="24" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" ht="24" customHeight="1">
-      <c r="A17" s="4" t="s">
+    <row r="18" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="24" customHeight="1">
-      <c r="A18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="3" t="s">
+    </row>
+    <row r="19" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="24" customHeight="1">
-      <c r="A19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="3" t="s">
+    </row>
+    <row r="20" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="24" customHeight="1">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="3" t="s">
+    </row>
+    <row r="21" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="24" customHeight="1">
-      <c r="A21" s="2" t="s">
+      <c r="B21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="3" t="s">
+    </row>
+    <row r="22" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="24" customHeight="1">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="24" customHeight="1">
-      <c r="A23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="3" t="s">
+    </row>
+    <row r="24" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="24" customHeight="1">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="3" t="s">
+    </row>
+    <row r="25" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="3" t="s">
+    </row>
+    <row r="26" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A26" s="4" t="s">
+      <c r="B26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="3" t="s">
+    </row>
+    <row r="27" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="3" t="s">
+    </row>
+    <row r="28" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="3" t="s">
+    </row>
+    <row r="29" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A29" s="4" t="s">
+      <c r="B29" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="3" t="s">
+    </row>
+    <row r="31" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="3" t="s">
+    </row>
+    <row r="32" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="3" t="s">
+    </row>
+    <row r="33" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="19.95" customHeight="1">
-      <c r="A33" s="7" t="s">
+      <c r="B33" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="3" t="s">
+    </row>
+    <row r="34" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="19.95" customHeight="1">
-      <c r="A34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="19.95" customHeight="1"/>
-    <row r="36" spans="1:2" ht="19.95" customHeight="1"/>
-    <row r="37" spans="1:2" ht="19.95" customHeight="1"/>
-    <row r="38" spans="1:2" ht="19.95" customHeight="1"/>
-    <row r="39" spans="1:2" ht="19.95" customHeight="1"/>
-    <row r="40" spans="1:2" ht="19.95" customHeight="1"/>
-    <row r="41" spans="1:2" ht="19.95" customHeight="1"/>
+    </row>
+    <row r="35" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>